<commit_message>
control flow assignment - for loop added
</commit_message>
<xml_diff>
--- a/React B10 G1.xlsx
+++ b/React B10 G1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashaa\Desktop\codemind\javascript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6614A43-6AF7-40CC-A784-1C44D0703E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC36CCD8-5125-409B-9203-A8D7350EDEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
@@ -28,11 +28,26 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>Ashaa</author>
     <author>Microsoft Office User</author>
-    <author>Ashaa</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{4B76430F-036D-0545-BD86-7FF3E142D70F}">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{9BCC6638-72D2-4E91-97D4-C25F4A41A6FF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Electricity cut 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="1" shapeId="0" xr:uid="{4B76430F-036D-0545-BD86-7FF3E142D70F}">
       <text>
         <r>
           <rPr>
@@ -47,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="1" shapeId="0" xr:uid="{26B56075-E19D-462B-862C-DA9D9FCA9346}">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{26B56075-E19D-462B-862C-DA9D9FCA9346}">
       <text>
         <r>
           <rPr>
@@ -66,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
   <si>
     <t>Student Name</t>
   </si>
@@ -99,6 +114,9 @@
   </si>
   <si>
     <t>Neha</t>
+  </si>
+  <si>
+    <t>Absent</t>
   </si>
 </sst>
 </file>
@@ -512,7 +530,7 @@
   <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -534,8 +552,12 @@
       <c r="D1" s="4">
         <v>45294</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="E1" s="4">
+        <v>45295</v>
+      </c>
+      <c r="F1" s="4">
+        <v>45296</v>
+      </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -564,8 +586,12 @@
       <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -594,8 +620,12 @@
       <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -624,8 +654,12 @@
       <c r="D4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -654,8 +688,12 @@
       <c r="D5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -684,8 +722,12 @@
       <c r="D6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -708,7 +750,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E6" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:F6" xr:uid="{F036FACA-372A-8349-BD3D-950830E988A4}">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>